<commit_message>
include luqman punya muet
</commit_message>
<xml_diff>
--- a/resources/excel/importExcelFiles/MUET.xlsx
+++ b/resources/excel/importExcelFiles/MUET.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="276">
   <si>
     <t>KOMPONEN KERTAS</t>
   </si>
@@ -806,11 +806,50 @@
   <si>
     <t>MM2103/3024</t>
   </si>
+  <si>
+    <t>MUHAMMAD LUQMAN HAKIM BIN ROHAIZI</t>
+  </si>
+  <si>
+    <t>991006-05-5193</t>
+  </si>
+  <si>
+    <t>ME1234/5678</t>
+  </si>
+  <si>
+    <t>MUET SESSION 1 2005</t>
+  </si>
+  <si>
+    <t>ME1234/5679</t>
+  </si>
+  <si>
+    <t>ME1234/5680</t>
+  </si>
+  <si>
+    <t>ME1234/5681</t>
+  </si>
+  <si>
+    <t>ME1234/5682</t>
+  </si>
+  <si>
+    <t>MUET SESSION 2 2018</t>
+  </si>
+  <si>
+    <t>ME1234/5683</t>
+  </si>
+  <si>
+    <t>MUET SESSION 2 2005</t>
+  </si>
+  <si>
+    <t>ME1234/5684</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="d mmmm yyyy"/>
+  </numFmts>
   <fonts count="3">
     <font>
       <sz val="11.0"/>
@@ -830,12 +869,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -844,7 +889,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -856,6 +901,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -7536,228 +7588,484 @@
       <c r="Z108" s="1"/>
     </row>
     <row r="109" ht="12.75" customHeight="1">
-      <c r="A109" s="1"/>
-      <c r="B109" s="1"/>
-      <c r="C109" s="1"/>
-      <c r="D109" s="1"/>
-      <c r="E109" s="1"/>
-      <c r="F109" s="1"/>
-      <c r="G109" s="1"/>
-      <c r="H109" s="1"/>
-      <c r="I109" s="1"/>
-      <c r="J109" s="1"/>
-      <c r="K109" s="1"/>
-      <c r="L109" s="1"/>
-      <c r="M109" s="1"/>
-      <c r="N109" s="1"/>
-      <c r="O109" s="1"/>
-      <c r="P109" s="1"/>
-      <c r="Q109" s="1"/>
-      <c r="R109" s="1"/>
-      <c r="S109" s="1"/>
-      <c r="T109" s="1"/>
-      <c r="U109" s="1"/>
-      <c r="V109" s="1"/>
-      <c r="W109" s="1"/>
-      <c r="X109" s="1"/>
-      <c r="Y109" s="1"/>
-      <c r="Z109" s="1"/>
+      <c r="A109" s="5">
+        <v>2023.0</v>
+      </c>
+      <c r="B109" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="C109" s="5">
+        <v>4184841.0</v>
+      </c>
+      <c r="D109" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E109" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="F109" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="G109" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="H109" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="I109" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J109" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K109" s="5">
+        <v>75.0</v>
+      </c>
+      <c r="L109" s="5">
+        <v>64.0</v>
+      </c>
+      <c r="M109" s="5">
+        <v>68.0</v>
+      </c>
+      <c r="N109" s="5">
+        <v>38.0</v>
+      </c>
+      <c r="O109" s="5">
+        <v>245.0</v>
+      </c>
+      <c r="P109" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q109" s="5"/>
+      <c r="R109" s="5"/>
+      <c r="S109" s="5"/>
+      <c r="T109" s="5"/>
+      <c r="U109" s="5"/>
+      <c r="V109" s="5"/>
+      <c r="W109" s="5"/>
+      <c r="X109" s="5"/>
+      <c r="Y109" s="5"/>
+      <c r="Z109" s="5"/>
     </row>
     <row r="110" ht="12.75" customHeight="1">
-      <c r="A110" s="1"/>
-      <c r="B110" s="1"/>
-      <c r="C110" s="1"/>
-      <c r="D110" s="1"/>
-      <c r="E110" s="1"/>
-      <c r="F110" s="1"/>
-      <c r="G110" s="1"/>
-      <c r="H110" s="1"/>
-      <c r="I110" s="1"/>
-      <c r="J110" s="1"/>
-      <c r="K110" s="1"/>
-      <c r="L110" s="1"/>
-      <c r="M110" s="1"/>
-      <c r="N110" s="1"/>
-      <c r="O110" s="1"/>
-      <c r="P110" s="1"/>
-      <c r="Q110" s="1"/>
-      <c r="R110" s="1"/>
-      <c r="S110" s="1"/>
-      <c r="T110" s="1"/>
-      <c r="U110" s="1"/>
-      <c r="V110" s="1"/>
-      <c r="W110" s="1"/>
-      <c r="X110" s="1"/>
-      <c r="Y110" s="1"/>
-      <c r="Z110" s="1"/>
+      <c r="A110" s="6">
+        <v>2018.0</v>
+      </c>
+      <c r="B110" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="C110" s="5">
+        <v>3726842.0</v>
+      </c>
+      <c r="D110" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="E110" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="F110" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="G110" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="H110" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="I110" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="J110" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="K110" s="5">
+        <v>32.0</v>
+      </c>
+      <c r="L110" s="5">
+        <v>31.0</v>
+      </c>
+      <c r="M110" s="5">
+        <v>77.0</v>
+      </c>
+      <c r="N110" s="5">
+        <v>55.0</v>
+      </c>
+      <c r="O110" s="5">
+        <v>195.0</v>
+      </c>
+      <c r="P110" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q110" s="5"/>
+      <c r="R110" s="5"/>
+      <c r="S110" s="5"/>
+      <c r="T110" s="5"/>
+      <c r="U110" s="5"/>
+      <c r="V110" s="5"/>
+      <c r="W110" s="5"/>
+      <c r="X110" s="5"/>
+      <c r="Y110" s="5"/>
+      <c r="Z110" s="5"/>
     </row>
     <row r="111" ht="12.75" customHeight="1">
-      <c r="A111" s="1"/>
-      <c r="B111" s="1"/>
-      <c r="C111" s="1"/>
-      <c r="D111" s="1"/>
-      <c r="E111" s="1"/>
-      <c r="F111" s="1"/>
-      <c r="G111" s="1"/>
-      <c r="H111" s="1"/>
-      <c r="I111" s="1"/>
-      <c r="J111" s="1"/>
-      <c r="K111" s="1"/>
-      <c r="L111" s="1"/>
-      <c r="M111" s="1"/>
-      <c r="N111" s="1"/>
-      <c r="O111" s="1"/>
-      <c r="P111" s="1"/>
-      <c r="Q111" s="1"/>
-      <c r="R111" s="1"/>
-      <c r="S111" s="1"/>
-      <c r="T111" s="1"/>
-      <c r="U111" s="1"/>
-      <c r="V111" s="1"/>
-      <c r="W111" s="1"/>
-      <c r="X111" s="1"/>
-      <c r="Y111" s="1"/>
-      <c r="Z111" s="1"/>
+      <c r="A111" s="6">
+        <v>2005.0</v>
+      </c>
+      <c r="B111" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="C111" s="5">
+        <v>3726842.0</v>
+      </c>
+      <c r="D111" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="E111" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="F111" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="G111" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="H111" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="I111" s="7">
+        <v>38511.0</v>
+      </c>
+      <c r="J111" s="7">
+        <v>40336.0</v>
+      </c>
+      <c r="K111" s="5">
+        <v>72.0</v>
+      </c>
+      <c r="L111" s="5">
+        <v>56.0</v>
+      </c>
+      <c r="M111" s="5">
+        <v>79.0</v>
+      </c>
+      <c r="N111" s="5">
+        <v>62.0</v>
+      </c>
+      <c r="O111" s="5">
+        <v>269.0</v>
+      </c>
+      <c r="P111" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q111" s="5"/>
+      <c r="R111" s="5"/>
+      <c r="S111" s="5"/>
+      <c r="T111" s="5"/>
+      <c r="U111" s="5"/>
+      <c r="V111" s="5"/>
+      <c r="W111" s="5"/>
+      <c r="X111" s="5"/>
+      <c r="Y111" s="5"/>
+      <c r="Z111" s="5"/>
     </row>
     <row r="112" ht="12.75" customHeight="1">
-      <c r="A112" s="1"/>
-      <c r="B112" s="1"/>
-      <c r="C112" s="1"/>
-      <c r="D112" s="1"/>
-      <c r="E112" s="1"/>
-      <c r="F112" s="1"/>
-      <c r="G112" s="1"/>
-      <c r="H112" s="1"/>
-      <c r="I112" s="1"/>
-      <c r="J112" s="1"/>
-      <c r="K112" s="1"/>
-      <c r="L112" s="1"/>
-      <c r="M112" s="1"/>
-      <c r="N112" s="1"/>
-      <c r="O112" s="1"/>
-      <c r="P112" s="1"/>
-      <c r="Q112" s="1"/>
-      <c r="R112" s="1"/>
-      <c r="S112" s="1"/>
-      <c r="T112" s="1"/>
-      <c r="U112" s="1"/>
-      <c r="V112" s="1"/>
-      <c r="W112" s="1"/>
-      <c r="X112" s="1"/>
-      <c r="Y112" s="1"/>
-      <c r="Z112" s="1"/>
+      <c r="A112" s="5">
+        <v>2023.0</v>
+      </c>
+      <c r="B112" s="6">
+        <v>2.0</v>
+      </c>
+      <c r="C112" s="5">
+        <v>4184841.0</v>
+      </c>
+      <c r="D112" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="E112" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="F112" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="G112" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="H112" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="I112" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J112" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K112" s="5">
+        <v>-1.0</v>
+      </c>
+      <c r="L112" s="5">
+        <v>-1.0</v>
+      </c>
+      <c r="M112" s="5">
+        <v>-1.0</v>
+      </c>
+      <c r="N112" s="5">
+        <v>-1.0</v>
+      </c>
+      <c r="O112" s="5">
+        <v>-1.0</v>
+      </c>
+      <c r="P112" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q112" s="5"/>
+      <c r="R112" s="5"/>
+      <c r="S112" s="5"/>
+      <c r="T112" s="5"/>
+      <c r="U112" s="5"/>
+      <c r="V112" s="5"/>
+      <c r="W112" s="5"/>
+      <c r="X112" s="5"/>
+      <c r="Y112" s="5"/>
+      <c r="Z112" s="5"/>
     </row>
     <row r="113" ht="12.75" customHeight="1">
-      <c r="A113" s="1"/>
-      <c r="B113" s="1"/>
-      <c r="C113" s="1"/>
-      <c r="D113" s="1"/>
-      <c r="E113" s="1"/>
-      <c r="F113" s="1"/>
-      <c r="G113" s="1"/>
-      <c r="H113" s="1"/>
-      <c r="I113" s="1"/>
-      <c r="J113" s="1"/>
-      <c r="K113" s="1"/>
-      <c r="L113" s="1"/>
-      <c r="M113" s="1"/>
-      <c r="N113" s="1"/>
-      <c r="O113" s="1"/>
-      <c r="P113" s="1"/>
-      <c r="Q113" s="1"/>
-      <c r="R113" s="1"/>
-      <c r="S113" s="1"/>
-      <c r="T113" s="1"/>
-      <c r="U113" s="1"/>
-      <c r="V113" s="1"/>
-      <c r="W113" s="1"/>
-      <c r="X113" s="1"/>
-      <c r="Y113" s="1"/>
-      <c r="Z113" s="1"/>
+      <c r="A113" s="5">
+        <v>2022.0</v>
+      </c>
+      <c r="B113" s="6">
+        <v>2.0</v>
+      </c>
+      <c r="C113" s="5">
+        <v>3975790.0</v>
+      </c>
+      <c r="D113" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="E113" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="F113" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="G113" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="H113" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="I113" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="J113" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="K113" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="L113" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="M113" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="N113" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="O113" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="P113" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q113" s="5"/>
+      <c r="R113" s="5"/>
+      <c r="S113" s="5"/>
+      <c r="T113" s="5"/>
+      <c r="U113" s="5"/>
+      <c r="V113" s="5"/>
+      <c r="W113" s="5"/>
+      <c r="X113" s="5"/>
+      <c r="Y113" s="5"/>
+      <c r="Z113" s="5"/>
     </row>
     <row r="114" ht="12.75" customHeight="1">
-      <c r="A114" s="1"/>
-      <c r="B114" s="1"/>
-      <c r="C114" s="1"/>
-      <c r="D114" s="1"/>
-      <c r="E114" s="1"/>
-      <c r="F114" s="1"/>
-      <c r="G114" s="1"/>
-      <c r="H114" s="1"/>
-      <c r="I114" s="1"/>
-      <c r="J114" s="1"/>
-      <c r="K114" s="1"/>
-      <c r="L114" s="1"/>
-      <c r="M114" s="1"/>
-      <c r="N114" s="1"/>
-      <c r="O114" s="1"/>
-      <c r="P114" s="1"/>
-      <c r="Q114" s="1"/>
-      <c r="R114" s="1"/>
-      <c r="S114" s="1"/>
-      <c r="T114" s="1"/>
-      <c r="U114" s="1"/>
-      <c r="V114" s="1"/>
-      <c r="W114" s="1"/>
-      <c r="X114" s="1"/>
-      <c r="Y114" s="1"/>
-      <c r="Z114" s="1"/>
+      <c r="A114" s="5">
+        <v>2021.0</v>
+      </c>
+      <c r="B114" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="C114" s="5">
+        <v>3858125.0</v>
+      </c>
+      <c r="D114" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="E114" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="F114" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="G114" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="H114" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="I114" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="J114" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="K114" s="6">
+        <v>-3.0</v>
+      </c>
+      <c r="L114" s="6">
+        <v>-3.0</v>
+      </c>
+      <c r="M114" s="6">
+        <v>-3.0</v>
+      </c>
+      <c r="N114" s="6">
+        <v>-3.0</v>
+      </c>
+      <c r="O114" s="6">
+        <v>-3.0</v>
+      </c>
+      <c r="P114" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q114" s="5"/>
+      <c r="R114" s="5"/>
+      <c r="S114" s="5"/>
+      <c r="T114" s="5"/>
+      <c r="U114" s="5"/>
+      <c r="V114" s="5"/>
+      <c r="W114" s="5"/>
+      <c r="X114" s="5"/>
+      <c r="Y114" s="5"/>
+      <c r="Z114" s="5"/>
     </row>
     <row r="115" ht="12.75" customHeight="1">
-      <c r="A115" s="1"/>
-      <c r="B115" s="1"/>
-      <c r="C115" s="1"/>
-      <c r="D115" s="1"/>
-      <c r="E115" s="1"/>
-      <c r="F115" s="1"/>
-      <c r="G115" s="1"/>
-      <c r="H115" s="1"/>
-      <c r="I115" s="1"/>
-      <c r="J115" s="1"/>
-      <c r="K115" s="1"/>
-      <c r="L115" s="1"/>
-      <c r="M115" s="1"/>
-      <c r="N115" s="1"/>
-      <c r="O115" s="1"/>
-      <c r="P115" s="1"/>
-      <c r="Q115" s="1"/>
-      <c r="R115" s="1"/>
-      <c r="S115" s="1"/>
-      <c r="T115" s="1"/>
-      <c r="U115" s="1"/>
-      <c r="V115" s="1"/>
-      <c r="W115" s="1"/>
-      <c r="X115" s="1"/>
-      <c r="Y115" s="1"/>
-      <c r="Z115" s="1"/>
+      <c r="A115" s="6">
+        <v>2018.0</v>
+      </c>
+      <c r="B115" s="6">
+        <v>2.0</v>
+      </c>
+      <c r="C115" s="5">
+        <v>3726842.0</v>
+      </c>
+      <c r="D115" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="E115" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="F115" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="G115" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="H115" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="I115" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="J115" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="K115" s="6">
+        <v>-4.0</v>
+      </c>
+      <c r="L115" s="6">
+        <v>-4.0</v>
+      </c>
+      <c r="M115" s="6">
+        <v>-4.0</v>
+      </c>
+      <c r="N115" s="6">
+        <v>-4.0</v>
+      </c>
+      <c r="O115" s="6">
+        <v>-4.0</v>
+      </c>
+      <c r="P115" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q115" s="5"/>
+      <c r="R115" s="5"/>
+      <c r="S115" s="5"/>
+      <c r="T115" s="5"/>
+      <c r="U115" s="5"/>
+      <c r="V115" s="5"/>
+      <c r="W115" s="5"/>
+      <c r="X115" s="5"/>
+      <c r="Y115" s="5"/>
+      <c r="Z115" s="5"/>
     </row>
     <row r="116" ht="12.75" customHeight="1">
-      <c r="A116" s="1"/>
-      <c r="B116" s="1"/>
-      <c r="C116" s="1"/>
-      <c r="D116" s="1"/>
-      <c r="E116" s="1"/>
-      <c r="F116" s="1"/>
-      <c r="G116" s="1"/>
-      <c r="H116" s="1"/>
-      <c r="I116" s="1"/>
-      <c r="J116" s="1"/>
-      <c r="K116" s="1"/>
-      <c r="L116" s="1"/>
-      <c r="M116" s="1"/>
-      <c r="N116" s="1"/>
-      <c r="O116" s="1"/>
-      <c r="P116" s="1"/>
-      <c r="Q116" s="1"/>
-      <c r="R116" s="1"/>
-      <c r="S116" s="1"/>
-      <c r="T116" s="1"/>
-      <c r="U116" s="1"/>
-      <c r="V116" s="1"/>
-      <c r="W116" s="1"/>
-      <c r="X116" s="1"/>
-      <c r="Y116" s="1"/>
-      <c r="Z116" s="1"/>
+      <c r="A116" s="6">
+        <v>2005.0</v>
+      </c>
+      <c r="B116" s="6">
+        <v>2.0</v>
+      </c>
+      <c r="C116" s="5">
+        <v>3726842.0</v>
+      </c>
+      <c r="D116" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="E116" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="F116" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="G116" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="H116" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="I116" s="7">
+        <v>38511.0</v>
+      </c>
+      <c r="J116" s="7">
+        <v>40336.0</v>
+      </c>
+      <c r="K116" s="6">
+        <v>-5.0</v>
+      </c>
+      <c r="L116" s="6">
+        <v>-5.0</v>
+      </c>
+      <c r="M116" s="6">
+        <v>-5.0</v>
+      </c>
+      <c r="N116" s="6">
+        <v>-5.0</v>
+      </c>
+      <c r="O116" s="6">
+        <v>-5.0</v>
+      </c>
+      <c r="P116" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q116" s="5"/>
+      <c r="R116" s="5"/>
+      <c r="S116" s="5"/>
+      <c r="T116" s="5"/>
+      <c r="U116" s="5"/>
+      <c r="V116" s="5"/>
+      <c r="W116" s="5"/>
+      <c r="X116" s="5"/>
+      <c r="Y116" s="5"/>
+      <c r="Z116" s="5"/>
     </row>
     <row r="117" ht="12.75" customHeight="1">
       <c r="A117" s="1"/>
@@ -32511,6 +32819,90 @@
       <c r="Y1000" s="1"/>
       <c r="Z1000" s="1"/>
     </row>
+    <row r="1001" ht="12.75" customHeight="1">
+      <c r="A1001" s="1"/>
+      <c r="B1001" s="1"/>
+      <c r="C1001" s="1"/>
+      <c r="D1001" s="1"/>
+      <c r="E1001" s="1"/>
+      <c r="F1001" s="1"/>
+      <c r="G1001" s="1"/>
+      <c r="H1001" s="1"/>
+      <c r="I1001" s="1"/>
+      <c r="J1001" s="1"/>
+      <c r="K1001" s="1"/>
+      <c r="L1001" s="1"/>
+      <c r="M1001" s="1"/>
+      <c r="N1001" s="1"/>
+      <c r="O1001" s="1"/>
+      <c r="P1001" s="1"/>
+      <c r="Q1001" s="1"/>
+      <c r="R1001" s="1"/>
+      <c r="S1001" s="1"/>
+      <c r="T1001" s="1"/>
+      <c r="U1001" s="1"/>
+      <c r="V1001" s="1"/>
+      <c r="W1001" s="1"/>
+      <c r="X1001" s="1"/>
+      <c r="Y1001" s="1"/>
+      <c r="Z1001" s="1"/>
+    </row>
+    <row r="1002" ht="12.75" customHeight="1">
+      <c r="A1002" s="1"/>
+      <c r="B1002" s="1"/>
+      <c r="C1002" s="1"/>
+      <c r="D1002" s="1"/>
+      <c r="E1002" s="1"/>
+      <c r="F1002" s="1"/>
+      <c r="G1002" s="1"/>
+      <c r="H1002" s="1"/>
+      <c r="I1002" s="1"/>
+      <c r="J1002" s="1"/>
+      <c r="K1002" s="1"/>
+      <c r="L1002" s="1"/>
+      <c r="M1002" s="1"/>
+      <c r="N1002" s="1"/>
+      <c r="O1002" s="1"/>
+      <c r="P1002" s="1"/>
+      <c r="Q1002" s="1"/>
+      <c r="R1002" s="1"/>
+      <c r="S1002" s="1"/>
+      <c r="T1002" s="1"/>
+      <c r="U1002" s="1"/>
+      <c r="V1002" s="1"/>
+      <c r="W1002" s="1"/>
+      <c r="X1002" s="1"/>
+      <c r="Y1002" s="1"/>
+      <c r="Z1002" s="1"/>
+    </row>
+    <row r="1003" ht="12.75" customHeight="1">
+      <c r="A1003" s="1"/>
+      <c r="B1003" s="1"/>
+      <c r="C1003" s="1"/>
+      <c r="D1003" s="1"/>
+      <c r="E1003" s="1"/>
+      <c r="F1003" s="1"/>
+      <c r="G1003" s="1"/>
+      <c r="H1003" s="1"/>
+      <c r="I1003" s="1"/>
+      <c r="J1003" s="1"/>
+      <c r="K1003" s="1"/>
+      <c r="L1003" s="1"/>
+      <c r="M1003" s="1"/>
+      <c r="N1003" s="1"/>
+      <c r="O1003" s="1"/>
+      <c r="P1003" s="1"/>
+      <c r="Q1003" s="1"/>
+      <c r="R1003" s="1"/>
+      <c r="S1003" s="1"/>
+      <c r="T1003" s="1"/>
+      <c r="U1003" s="1"/>
+      <c r="V1003" s="1"/>
+      <c r="W1003" s="1"/>
+      <c r="X1003" s="1"/>
+      <c r="Y1003" s="1"/>
+      <c r="Z1003" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="K1:N1"/>

</xml_diff>